<commit_message>
testing 222_2, found training x number is larger than the old one
</commit_message>
<xml_diff>
--- a/reports/Results_table.xlsx
+++ b/reports/Results_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hp/GitHub/EEG/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C0306F-68E0-4245-8354-814C86A1BB47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38574E03-2530-0F4A-AEB1-1D2BFDAEC914}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="2940" windowWidth="27640" windowHeight="16940" xr2:uid="{BA87DAA3-A384-EB4A-8863-C5C6B40D54ED}"/>
+    <workbookView xWindow="3260" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{BA87DAA3-A384-EB4A-8863-C5C6B40D54ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Settings/Patients</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>90 without delta</t>
+  </si>
+  <si>
+    <t>124 with delta no</t>
   </si>
 </sst>
 </file>
@@ -65,12 +68,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,10 +94,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B83447A-83E2-6F4B-8CB1-91BD9B1562E7}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,63 +448,62 @@
     </row>
     <row r="2" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>88.77</v>
-      </c>
-      <c r="C2" s="2">
-        <v>75.34</v>
-      </c>
-      <c r="D2" s="2">
-        <v>70.150000000000006</v>
-      </c>
-      <c r="E2" s="2">
-        <v>81.58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>89.14</v>
+        <v>88.77</v>
       </c>
       <c r="C3" s="2">
-        <v>72.849999999999994</v>
-      </c>
-      <c r="D3" s="2">
-        <v>70.44</v>
-      </c>
-      <c r="E3" s="2">
-        <v>80.16</v>
+        <v>75.34</v>
+      </c>
+      <c r="D3" s="3">
+        <v>70.150000000000006</v>
+      </c>
+      <c r="E3" s="3">
+        <v>81.58</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>88.54</v>
+        <v>89.14</v>
       </c>
       <c r="C4" s="2">
-        <v>73.47</v>
-      </c>
-      <c r="D4" s="2">
-        <v>70.260000000000005</v>
-      </c>
-      <c r="E4" s="2">
-        <v>80</v>
+        <v>72.849999999999994</v>
+      </c>
+      <c r="D4" s="3">
+        <v>70.44</v>
+      </c>
+      <c r="E4" s="3">
+        <v>80.16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>88.54</v>
+      </c>
+      <c r="C5" s="2">
+        <v>73.47</v>
+      </c>
+      <c r="D5" s="3">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="E5" s="3">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tried new split, tried weekly epoch, ready to try new random seed
</commit_message>
<xml_diff>
--- a/reports/Results_table.xlsx
+++ b/reports/Results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hp/GitHub/EEG/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38574E03-2530-0F4A-AEB1-1D2BFDAEC914}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A60434-0E4F-0448-98F7-29C694F6BAA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{BA87DAA3-A384-EB4A-8863-C5C6B40D54ED}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Settings/Patients</t>
   </si>
@@ -42,17 +47,23 @@
     <t>124 without delta</t>
   </si>
   <si>
-    <t>90 without delta</t>
-  </si>
-  <si>
-    <t>124 with delta no</t>
+    <t>Original monthly epoch, original Python split (90 without delta)</t>
+  </si>
+  <si>
+    <t>Original monthly epoch, NEW even split</t>
+  </si>
+  <si>
+    <t>NEW weekly epoch, NEW even split</t>
+  </si>
+  <si>
+    <t>NEW biweekly epoch, NEW even split</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,8 +78,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +96,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -94,15 +118,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,90 +451,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B83447A-83E2-6F4B-8CB1-91BD9B1562E7}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.83203125" style="8" customWidth="1"/>
     <col min="2" max="5" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>231</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
+        <v>241</v>
+      </c>
+      <c r="L1" s="1">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>88.77</v>
+      </c>
+      <c r="C2" s="2">
+        <v>75.34</v>
+      </c>
+      <c r="D2" s="2">
+        <v>70.150000000000006</v>
+      </c>
+      <c r="E2" s="2">
+        <v>87.87</v>
+      </c>
+      <c r="L2" s="2">
+        <v>83.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>89.14</v>
+      </c>
+      <c r="C3" s="2">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="D3" s="2">
+        <v>70.44</v>
+      </c>
+      <c r="L3" s="2">
+        <v>83.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>88.54</v>
+      </c>
+      <c r="C4" s="5">
+        <v>73.47</v>
+      </c>
+      <c r="D4" s="5">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="E4" s="5">
+        <v>87.87</v>
+      </c>
+      <c r="L4" s="5">
+        <v>83.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>88.77</v>
-      </c>
-      <c r="C3" s="2">
-        <v>75.34</v>
-      </c>
-      <c r="D3" s="3">
-        <v>70.150000000000006</v>
-      </c>
-      <c r="E3" s="3">
-        <v>81.58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>89.14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>72.849999999999994</v>
-      </c>
-      <c r="D4" s="3">
-        <v>70.44</v>
-      </c>
-      <c r="E4" s="3">
-        <v>80.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>88.54</v>
-      </c>
-      <c r="C5" s="2">
-        <v>73.47</v>
+      <c r="B5" s="1">
+        <v>83.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>65.900000000000006</v>
       </c>
       <c r="D5" s="3">
-        <v>70.260000000000005</v>
+        <v>77.25</v>
       </c>
       <c r="E5" s="3">
-        <v>80</v>
-      </c>
+        <v>87.84</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>60.94</v>
+      </c>
+      <c r="C7" s="1">
+        <v>73.78</v>
+      </c>
+      <c r="D7" s="3">
+        <v>59.3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>72.22</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>66.58</v>
+      </c>
+      <c r="C8" s="1">
+        <v>72.73</v>
+      </c>
+      <c r="D8" s="3">
+        <v>70.25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>87.74</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran the different random seed, add the option to not use absolute value for the feature importance function
</commit_message>
<xml_diff>
--- a/reports/Results_table.xlsx
+++ b/reports/Results_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hp/GitHub/EEG/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A60434-0E4F-0448-98F7-29C694F6BAA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA3D711-AFE4-074C-AAC5-0F086D704F19}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{BA87DAA3-A384-EB4A-8863-C5C6B40D54ED}"/>
+    <workbookView xWindow="3560" yWindow="2140" windowWidth="27640" windowHeight="16940" xr2:uid="{BA87DAA3-A384-EB4A-8863-C5C6B40D54ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Settings/Patients</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>NEW biweekly epoch, NEW even split</t>
+  </si>
+  <si>
+    <t>Original monthly epoch, old split, random seed = 11</t>
+  </si>
+  <si>
+    <t>Original monthly epoch, old split, random seed = 77</t>
+  </si>
+  <si>
+    <t>Original monthly epoch, old split, random seed = 93</t>
   </si>
 </sst>
 </file>
@@ -454,7 +463,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D41" sqref="D29:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -614,26 +623,59 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>83.19</v>
+      </c>
+      <c r="C10" s="1">
+        <v>73.37</v>
+      </c>
+      <c r="D10" s="3">
+        <v>59.83</v>
+      </c>
+      <c r="E10" s="3">
+        <v>72.599999999999994</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>85.04</v>
+      </c>
+      <c r="C11" s="1">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="D11" s="3">
+        <v>68.27</v>
+      </c>
+      <c r="E11" s="3">
+        <v>89.87</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>85.12</v>
+      </c>
+      <c r="C12" s="1">
+        <v>69.19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="E12" s="3">
+        <v>83.87</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>

</xml_diff>